<commit_message>
corrected file names to conform to standard, corrected preparer name to conform to standard
</commit_message>
<xml_diff>
--- a/library/library_hbrown_05.25.20.xlsx
+++ b/library/library_hbrown_05.25.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF7E6A65-DCE2-3D41-8576-2A7C835AAB41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7D17BA-C5A4-E24E-913B-5DDD1C6956AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{60A1E46A-5C4F-014F-99FE-D6C92F91B89F}"/>
+    <workbookView xWindow="6440" yWindow="520" windowWidth="18580" windowHeight="16940" xr2:uid="{60A1E46A-5C4F-014F-99FE-D6C92F91B89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>05.25.20</t>
   </si>
   <si>
-    <t>H.Brown</t>
-  </si>
-  <si>
     <t>Index1_1</t>
   </si>
   <si>
@@ -235,16 +232,26 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>H.BROWN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,9 +277,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +598,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,8 +645,8 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -646,37 +654,37 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
+      <c r="E2" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -684,37 +692,37 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="E3" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="B4" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -722,37 +730,37 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
+      <c r="B5" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -760,37 +768,37 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
+      <c r="B6" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -798,37 +806,37 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
+      <c r="E6" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
+      <c r="B7" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -836,37 +844,37 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
+      <c r="E7" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
+      <c r="B8" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -874,37 +882,37 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
-        <v>13</v>
+      <c r="E8" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
       <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
         <v>29</v>
       </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
+      <c r="B9" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -912,37 +920,37 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
-        <v>13</v>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
       <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
       </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -950,37 +958,37 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>13</v>
+      <c r="E10" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
+      <c r="B11" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -988,37 +996,37 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
-        <v>13</v>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
         <v>35</v>
       </c>
-      <c r="H11" t="s">
-        <v>36</v>
-      </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
+      <c r="B12" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -1026,37 +1034,37 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
-        <v>13</v>
+      <c r="E12" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
       <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
         <v>37</v>
       </c>
-      <c r="H12" t="s">
-        <v>38</v>
-      </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
+      <c r="B13" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -1064,37 +1072,37 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>13</v>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
         <v>39</v>
       </c>
-      <c r="H13" t="s">
-        <v>40</v>
-      </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
+      <c r="B14" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -1102,37 +1110,37 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
-        <v>13</v>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
         <v>41</v>
       </c>
-      <c r="H14" t="s">
-        <v>42</v>
-      </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -1140,37 +1148,37 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
-        <v>13</v>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
         <v>43</v>
       </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
-        <v>13</v>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1178,37 +1186,37 @@
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" t="s">
-        <v>13</v>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
         <v>45</v>
       </c>
-      <c r="H16" t="s">
-        <v>46</v>
-      </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
-        <v>13</v>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -1216,37 +1224,37 @@
       <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" t="s">
-        <v>13</v>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F17">
         <v>16</v>
       </c>
       <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
         <v>47</v>
       </c>
-      <c r="H17" t="s">
-        <v>48</v>
-      </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" t="s">
-        <v>13</v>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -1254,37 +1262,37 @@
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
-        <v>13</v>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
       <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
         <v>49</v>
       </c>
-      <c r="H18" t="s">
-        <v>50</v>
-      </c>
       <c r="I18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
-        <v>13</v>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -1292,37 +1300,37 @@
       <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="E19" t="s">
-        <v>13</v>
+      <c r="E19" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F19">
         <v>18</v>
       </c>
       <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
         <v>51</v>
       </c>
-      <c r="H19" t="s">
-        <v>52</v>
-      </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" t="s">
-        <v>13</v>
+      <c r="B20" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1330,37 +1338,37 @@
       <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="E20" t="s">
-        <v>13</v>
+      <c r="E20" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
       <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" t="s">
-        <v>54</v>
-      </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
-        <v>13</v>
+      <c r="B21" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1368,37 +1376,37 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="s">
-        <v>13</v>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
       <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
         <v>55</v>
       </c>
-      <c r="H21" t="s">
-        <v>56</v>
-      </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B22" t="s">
-        <v>13</v>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1406,37 +1414,37 @@
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E22" t="s">
-        <v>13</v>
+      <c r="E22" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" t="s">
         <v>57</v>
       </c>
-      <c r="H22" t="s">
-        <v>58</v>
-      </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
-        <v>13</v>
+      <c r="B23" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1444,37 +1452,37 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s">
-        <v>13</v>
+      <c r="E23" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F23">
         <v>22</v>
       </c>
       <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
         <v>59</v>
       </c>
-      <c r="H23" t="s">
-        <v>60</v>
-      </c>
       <c r="I23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" t="s">
-        <v>13</v>
+      <c r="B24" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1482,37 +1490,37 @@
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
-        <v>13</v>
+      <c r="E24" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F24">
         <v>23</v>
       </c>
       <c r="G24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" t="s">
         <v>61</v>
       </c>
-      <c r="H24" t="s">
-        <v>62</v>
-      </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
-        <v>13</v>
+      <c r="B25" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1520,37 +1528,37 @@
       <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="E25" t="s">
-        <v>13</v>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" t="s">
         <v>63</v>
       </c>
-      <c r="H25" t="s">
-        <v>64</v>
-      </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
-        <v>13</v>
+      <c r="B26" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1558,37 +1566,37 @@
       <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="E26" t="s">
-        <v>13</v>
+      <c r="E26" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F26">
         <v>25</v>
       </c>
       <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
         <v>65</v>
       </c>
-      <c r="H26" t="s">
-        <v>66</v>
-      </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
-        <v>13</v>
+      <c r="B27" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1596,29 +1604,29 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
-      <c r="E27" t="s">
-        <v>13</v>
+      <c r="E27" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F27">
         <v>26</v>
       </c>
       <c r="G27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" t="s">
         <v>67</v>
       </c>
-      <c r="H27" t="s">
-        <v>68</v>
-      </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>